<commit_message>
SacrificialStab and WickedStab Added and Working.
</commit_message>
<xml_diff>
--- a/Basegame Character Card Stats.xlsx
+++ b/Basegame Character Card Stats.xlsx
@@ -1,34 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20339"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Stuff\Coding\ModdingSlayTheSpire\my_mods\git\StS-DefaultModBase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SlaySpireMod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4D4958-2D4A-4279-92AE-904F3C9F1E52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FF9C83-622F-42B9-857D-8BF459AF80D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="278" xr2:uid="{AD2E1A73-3376-4E41-A344-6779F4DBBFBB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="278" activeTab="1" xr2:uid="{AD2E1A73-3376-4E41-A344-6779F4DBBFBB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_Hlk529464078" localSheetId="0">Sheet1!#REF!</definedName>
+    <definedName name="_Hlk529464078" localSheetId="1">Sheet1!#REF!</definedName>
+    <definedName name="_Hlk529464078" localSheetId="0">'Sheet1 (2)'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="21">
   <si>
     <t>Common</t>
   </si>
@@ -211,20 +224,8 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -237,15 +238,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -253,6 +245,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -264,7 +265,10 @@
     <cellStyle name="60% - Accent4" xfId="3" builtinId="44"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="62">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -288,15 +292,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -325,6 +320,21 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -344,15 +354,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -387,6 +388,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -406,21 +416,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -437,6 +432,198 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -483,8 +670,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Gremy Simple Dark" pivot="0" count="2" xr9:uid="{588A353C-8878-412F-8D27-6178F08779F5}">
-      <tableStyleElement type="wholeTable" dxfId="31"/>
-      <tableStyleElement type="headerRow" dxfId="30"/>
+      <tableStyleElement type="wholeTable" dxfId="61"/>
+      <tableStyleElement type="headerRow" dxfId="60"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -507,7 +694,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2121A485-2482-4860-9E30-DE2D287A6F7A}" name="Table2" displayName="Table2" ref="A6:D13" totalsRowCount="1" headerRowDxfId="29" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C4D8D86C-EF36-476A-960E-AE0225BCAD6C}" name="Table25" displayName="Table25" ref="A6:D13" totalsRowCount="1" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="A6:D12" xr:uid="{D21865EF-8925-4FB2-A04B-9FCEFE947069}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -515,17 +702,17 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{FF4810EE-C708-4E37-835D-7BB9DD96E48C}" name="Cost" totalsRowLabel="Total" dataDxfId="27" totalsRowDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{4B7223C6-8335-433A-9378-28EFCCDBF04D}" name="Silent" totalsRowFunction="sum" dataDxfId="26" totalsRowDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{2C581A80-D6F5-4915-9D06-BA8D353C068D}" name="Ironclad" totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{BA528A4A-ED02-4115-906A-32084823D809}" name="Defect" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{70F0183D-A823-4065-8446-A116DB0AE55A}" name="Cost" totalsRowLabel="Total" dataDxfId="26" totalsRowDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{E94D7627-C8A8-41D8-84B5-89B046242B3D}" name="Silent" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{F82F7625-583F-41B7-B0E1-8A356A339918}" name="Ironclad" totalsRowFunction="sum" dataDxfId="22" totalsRowDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{BF62A352-15C1-44F1-B4A1-C21BB4DDC948}" name="Defect" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="Gremy Simple Dark" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53B8ADF9-4707-47E1-BDFA-3F006EA823AB}" name="Table24" displayName="Table24" ref="F6:I11" totalsRowCount="1" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{97B47284-656F-4C63-B7A3-841E8AFD9751}" name="Table246" displayName="Table246" ref="F6:I11" totalsRowCount="1" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="F6:I10" xr:uid="{CE12703D-A0E8-4EAA-9688-E5928D5B5BFB}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -533,23 +720,72 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{28832C6B-C5A0-4B28-9B43-B972B39FC7E3}" name="Rarity" totalsRowLabel="Total" dataDxfId="21" totalsRowDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{BBDEB0D6-F456-42CF-9E45-0769D86C8EBC}" name="Silent" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{FE11044C-0B04-4341-B805-DD3FC475A98D}" name="Ironclad" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{3473F5BA-E9A0-42BC-A801-C0AA1A01137A}" name="Defect" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{4BA0275D-E925-4FBA-B354-D41E6DC9F334}" name="Rarity" totalsRowLabel="Total" dataDxfId="16" totalsRowDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{D1897B02-72AD-458B-B029-26D58A7647E2}" name="Silent" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{29DC924D-3CAA-4094-9D30-763785AFC677}" name="Ironclad" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{511F028A-E08D-41A9-A070-87A30F33218D}" name="Defect" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="Gremy Simple Dark" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9FEC834A-9605-4DAB-8FC8-559DFE95E7CE}" name="Table242" displayName="Table242" ref="F16:I20" totalsRowCount="1" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AC76064A-EB71-487D-8927-BA2141DDEA23}" name="Table2427" displayName="Table2427" ref="F16:I20" totalsRowCount="1" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="F16:I19" xr:uid="{AB9EBA6F-19E5-4878-B4BF-640070BDE1CB}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{10488BD1-9981-44C8-B679-8617EA80CFDF}" name="Type" totalsRowLabel="Total" dataDxfId="15" totalsRowDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{2BD6E313-819A-4120-B615-A73747A8BFF9}" name="Silent" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{29092D1A-1D35-4F6E-9938-E644E403DC81}" name="Ironclad" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{D8133038-6E03-4174-95AC-6C4D249B7298}" name="Defect" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{432BEE7C-30BD-4DC2-827C-434F72595DE4}" name="Type" totalsRowLabel="Total" dataDxfId="6" totalsRowDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{B069A842-EB3F-4E0C-84F6-E881F1D1CBAD}" name="Silent" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{781BE405-93EB-4032-8BAB-BC3DFE907808}" name="Ironclad" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{C33A31BC-AE30-43A3-9879-9BB7B4B7BEBC}" name="Defect" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="Gremy Simple Dark" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2121A485-2482-4860-9E30-DE2D287A6F7A}" name="Table2" displayName="Table2" ref="A6:D13" totalsRowCount="1" headerRowDxfId="59" dataDxfId="58">
+  <autoFilter ref="A6:D12" xr:uid="{D21865EF-8925-4FB2-A04B-9FCEFE947069}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{FF4810EE-C708-4E37-835D-7BB9DD96E48C}" name="Cost" totalsRowLabel="Total" dataDxfId="57" totalsRowDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{4B7223C6-8335-433A-9378-28EFCCDBF04D}" name="Silent" totalsRowFunction="sum" dataDxfId="55" totalsRowDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{2C581A80-D6F5-4915-9D06-BA8D353C068D}" name="Ironclad" totalsRowFunction="sum" dataDxfId="53" totalsRowDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{BA528A4A-ED02-4115-906A-32084823D809}" name="Defect" totalsRowFunction="sum" dataDxfId="51" totalsRowDxfId="50"/>
+  </tableColumns>
+  <tableStyleInfo name="Gremy Simple Dark" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53B8ADF9-4707-47E1-BDFA-3F006EA823AB}" name="Table24" displayName="Table24" ref="F6:I11" totalsRowCount="1" headerRowDxfId="49" dataDxfId="48">
+  <autoFilter ref="F6:I10" xr:uid="{CE12703D-A0E8-4EAA-9688-E5928D5B5BFB}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{28832C6B-C5A0-4B28-9B43-B972B39FC7E3}" name="Rarity" totalsRowLabel="Total" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{BBDEB0D6-F456-42CF-9E45-0769D86C8EBC}" name="Silent" totalsRowFunction="sum" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{FE11044C-0B04-4341-B805-DD3FC475A98D}" name="Ironclad" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{3473F5BA-E9A0-42BC-A801-C0AA1A01137A}" name="Defect" totalsRowFunction="sum" dataDxfId="41" totalsRowDxfId="40"/>
+  </tableColumns>
+  <tableStyleInfo name="Gremy Simple Dark" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9FEC834A-9605-4DAB-8FC8-559DFE95E7CE}" name="Table242" displayName="Table242" ref="F16:I20" totalsRowCount="1" headerRowDxfId="39" dataDxfId="38">
+  <autoFilter ref="F16:I19" xr:uid="{AB9EBA6F-19E5-4878-B4BF-640070BDE1CB}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{10488BD1-9981-44C8-B679-8617EA80CFDF}" name="Type" totalsRowLabel="Total" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{2BD6E313-819A-4120-B615-A73747A8BFF9}" name="Silent" totalsRowFunction="sum" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{29092D1A-1D35-4F6E-9938-E644E403DC81}" name="Ironclad" totalsRowFunction="sum" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{D8133038-6E03-4174-95AC-6C4D249B7298}" name="Defect" totalsRowFunction="sum" dataDxfId="31" totalsRowDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="Gremy Simple Dark" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -851,208 +1087,567 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7173905A-9702-4724-9D18-DFCD7AC58563}">
-  <dimension ref="A1:I30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{609CD6AD-2849-4D45-B4BD-E795C100316B}">
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="12.42578125" style="4"/>
+    <col min="1" max="16384" width="12.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="F5" s="9" t="s">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="F5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="1">
         <v>3</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="1">
         <v>3</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="1">
         <v>4</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="1">
         <v>3</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>0</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="1">
         <v>11</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="1">
         <v>12</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="1">
         <v>12</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="1">
         <v>19</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="1">
         <v>20</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>1</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="1">
         <v>42</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="1">
         <v>40</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="1">
         <v>43</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="1">
         <v>33</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="1">
         <v>36</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="1">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
         <v>2</v>
       </c>
       <c r="B10" s="1">
         <v>13</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>17</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="1">
         <v>11</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="1">
         <v>19</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="1">
         <v>16</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
         <v>3</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="1">
         <v>3</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>4</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="1">
         <v>4</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="1">
+        <f>SUBTOTAL(109,Table246[Silent])</f>
+        <v>75</v>
+      </c>
+      <c r="H11" s="1">
+        <f>SUBTOTAL(109,Table246[Ironclad])</f>
+        <v>75</v>
+      </c>
+      <c r="I11" s="1">
+        <f>SUBTOTAL(109,Table246[Defect])</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1">
+        <f>SUBTOTAL(109,Table25[Silent])</f>
+        <v>73</v>
+      </c>
+      <c r="C13" s="1">
+        <f>SUBTOTAL(109,Table25[Ironclad])</f>
+        <v>75</v>
+      </c>
+      <c r="D13" s="1">
+        <f>SUBTOTAL(109,Table25[Defect])</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="F15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="F16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="F17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="1">
+        <v>28</v>
+      </c>
+      <c r="H17" s="1">
+        <v>32</v>
+      </c>
+      <c r="I17" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F18" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="1">
+        <v>36</v>
+      </c>
+      <c r="H18" s="1">
+        <v>29</v>
+      </c>
+      <c r="I18" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="1">
+        <v>11</v>
+      </c>
+      <c r="H19" s="1">
+        <v>14</v>
+      </c>
+      <c r="I19" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="1">
+        <f>SUBTOTAL(109,Table2427[Silent])</f>
+        <v>75</v>
+      </c>
+      <c r="H20" s="1">
+        <f>SUBTOTAL(109,Table2427[Ironclad])</f>
+        <v>75</v>
+      </c>
+      <c r="I20" s="1">
+        <f>SUBTOTAL(109,Table2427[Defect])</f>
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:G3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="A15:D17"/>
+    <mergeCell ref="F15:I15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <tableParts count="3">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7173905A-9702-4724-9D18-DFCD7AC58563}">
+  <dimension ref="A1:I20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="12.44140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="F5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="1">
+        <v>4</v>
+      </c>
+      <c r="H7" s="1">
+        <v>3</v>
+      </c>
+      <c r="I7" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1">
+        <v>12</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>19</v>
+      </c>
+      <c r="H8" s="1">
+        <v>20</v>
+      </c>
+      <c r="I8" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1">
+        <v>42</v>
+      </c>
+      <c r="C9" s="1">
+        <v>40</v>
+      </c>
+      <c r="D9" s="1">
+        <v>43</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>33</v>
+      </c>
+      <c r="H9" s="1">
+        <v>36</v>
+      </c>
+      <c r="I9" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1">
+        <v>13</v>
+      </c>
+      <c r="C10" s="1">
+        <v>17</v>
+      </c>
+      <c r="D10" s="1">
+        <v>11</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>19</v>
+      </c>
+      <c r="H10" s="1">
+        <v>16</v>
+      </c>
+      <c r="I10" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1">
+        <v>4</v>
+      </c>
+      <c r="D11" s="1">
+        <v>4</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="1">
         <f>SUBTOTAL(109,Table24[Silent])</f>
         <v>75</v>
       </c>
@@ -1060,30 +1655,30 @@
         <f>SUBTOTAL(109,Table24[Ironclad])</f>
         <v>75</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="1">
         <f>SUBTOTAL(109,Table24[Defect])</f>
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>1</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>1</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="1">
         <f>SUBTOTAL(109,Table2[Silent])</f>
         <v>73</v>
       </c>
@@ -1091,100 +1686,94 @@
         <f>SUBTOTAL(109,Table2[Ironclad])</f>
         <v>75</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="1">
         <f>SUBTOTAL(109,Table2[Defect])</f>
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="F15" s="9" t="s">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="F15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="F16" s="4" t="s">
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="F16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I16" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="F17" s="12" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="F17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="1">
         <v>28</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="1">
         <v>32</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="1">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="F18" s="13" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F18" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="1">
         <v>36</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18" s="1">
         <v>29</v>
       </c>
-      <c r="I18" s="4">
+      <c r="I18" s="1">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="F19" s="14" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F19" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="1">
         <v>11</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H19" s="1">
         <v>14</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I19" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="F20" s="5" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="1">
         <f>SUBTOTAL(109,Table242[Silent])</f>
         <v>75</v>
       </c>
@@ -1192,28 +1781,10 @@
         <f>SUBTOTAL(109,Table242[Ironclad])</f>
         <v>75</v>
       </c>
-      <c r="I20" s="5">
+      <c r="I20" s="1">
         <f>SUBTOTAL(109,Table242[Defect])</f>
         <v>75</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G30" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>